<commit_message>
data added in sheet
</commit_message>
<xml_diff>
--- a/pageobjects/testData/files/usersCredentials.xlsx
+++ b/pageobjects/testData/files/usersCredentials.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>admin</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>ceyoyi9934@ptiong.com</t>
+  </si>
+  <si>
+    <t>FHDCMobileLogin</t>
+  </si>
+  <si>
+    <t>testcaregiver2may@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,6 +553,17 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>